<commit_message>
Starting show all results
</commit_message>
<xml_diff>
--- a/games_data.xlsx
+++ b/games_data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24131"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24228"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://masseyhighschoolnz-my.sharepoint.com/personal/alis70929_masseyhigh_school_nz/Documents/Old School Files/Documents/Com_201/02_Databases/01_DatabasePracticeTask/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="140" documentId="8_{131CAF5C-4678-441E-B044-CFE2BC2EDACB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7DF87D14-9002-4391-A811-61DB871E681F}"/>
+  <xr:revisionPtr revIDLastSave="142" documentId="8_{131CAF5C-4678-441E-B044-CFE2BC2EDACB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2554FC3C-74E2-4926-A885-FF09BA8D007F}"/>
   <bookViews>
-    <workbookView xWindow="-4560" yWindow="735" windowWidth="21600" windowHeight="11385" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1020" yWindow="1635" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Notes" sheetId="6" r:id="rId1"/>
@@ -5918,7 +5918,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:A19"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -16040,12 +16042,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4A3CF89C-E4BB-4AF5-AA41-5CF64189CFD0}">
   <dimension ref="A1:N249"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="A103" workbookViewId="0">
       <selection activeCell="J222" sqref="J222"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="2" max="2" width="19.42578125" customWidth="1"/>
     <col min="10" max="10" width="17.140625" customWidth="1"/>
     <col min="11" max="11" width="12.5703125" customWidth="1"/>
   </cols>

</xml_diff>